<commit_message>
DWH-11: Taxonomy service, fixes
</commit_message>
<xml_diff>
--- a/importer/src/test/resources/matrix.xlsx
+++ b/importer/src/test/resources/matrix.xlsx
@@ -28,16 +28,16 @@
     <t xml:space="preserve">supplierServiceType</t>
   </si>
   <si>
-    <t xml:space="preserve">taxonomyTypeLetter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taxonomyTypeParcel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taxonomyTypeLetterId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taxonomyTypeParcelId</t>
+    <t xml:space="preserve">standardServiceTypeLetter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standardServiceTypeParcel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standardServiceTypeLetterKey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standardServiceTypeParcelKey</t>
   </si>
   <si>
     <t xml:space="preserve">USPS</t>
@@ -479,15 +479,18 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="18.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
DWH-11: Add more assertions
</commit_message>
<xml_diff>
--- a/importer/src/test/resources/matrix.xlsx
+++ b/importer/src/test/resources/matrix.xlsx
@@ -208,22 +208,22 @@
     <t xml:space="preserve">FedEx</t>
   </si>
   <si>
-    <t xml:space="preserve">FedEx® Pak FedEx First Overnight®</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FedEx® Pak  FedEx Priority Overnight®</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FedEx® Pak FedEx Standard Overnight®</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FedEx® Pak FedEx 2Day® A.M.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FedEx® Pak FedEx 2Day®</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FedEx® Pak FedEx Express Saver®</t>
+    <t xml:space="preserve">FedEx® FedEx First Overnight®</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FedEx® FedEx Priority Overnight®</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FedEx® FedEx Standard Overnight®</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FedEx® FedEx 2Day® A.M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FedEx® FedEx 2Day®</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FedEx® FedEx Express Saver®</t>
   </si>
   <si>
     <t xml:space="preserve">FedEx® express Multiweight FedEx First Overnight®</t>
@@ -479,10 +479,10 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.47"/>

</xml_diff>